<commit_message>
MFY auto commit at 12/01/2022 19:55:38
</commit_message>
<xml_diff>
--- a/5) Data Communication and Networks_BM/Lab/Assignment/A/muhammadFahad_Assignmet.xlsx
+++ b/5) Data Communication and Networks_BM/Lab/Assignment/A/muhammadFahad_Assignmet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="360" windowWidth="16680" windowHeight="6900"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="16680" windowHeight="6900"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -97,7 +97,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="180" formatCode="0.0000E+00"/>
+    <numFmt numFmtId="164" formatCode="0.0000E+00"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -213,30 +213,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -244,15 +235,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -268,6 +250,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -553,22 +553,22 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:J6"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="18.7109375" style="1"/>
-    <col min="3" max="3" width="0" style="19" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" style="13" customWidth="1"/>
     <col min="4" max="4" width="18.7109375" style="1"/>
     <col min="5" max="5" width="18.7109375" style="1" customWidth="1"/>
     <col min="6" max="7" width="18.7109375" style="1"/>
-    <col min="8" max="8" width="29" style="16" customWidth="1"/>
+    <col min="8" max="8" width="29" style="10" customWidth="1"/>
     <col min="9" max="16384" width="18.7109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="13" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1">
@@ -579,7 +579,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="13" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="1">
@@ -588,7 +588,7 @@
       <c r="G2" s="1">
         <v>1</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="H2" s="10" t="s">
         <v>11</v>
       </c>
       <c r="I2" s="1" t="str">
@@ -601,7 +601,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="1">
@@ -610,7 +610,7 @@
       <c r="G3" s="1">
         <v>2</v>
       </c>
-      <c r="H3" s="16" t="s">
+      <c r="H3" s="10" t="s">
         <v>12</v>
       </c>
       <c r="I3" s="1" t="str">
@@ -626,7 +626,7 @@
       <c r="G4" s="1">
         <v>3</v>
       </c>
-      <c r="H4" s="16" t="s">
+      <c r="H4" s="10" t="s">
         <v>13</v>
       </c>
       <c r="I4" s="1" t="str">
@@ -642,7 +642,7 @@
       <c r="G5" s="1">
         <v>4</v>
       </c>
-      <c r="H5" s="16" t="s">
+      <c r="H5" s="10" t="s">
         <v>14</v>
       </c>
       <c r="I5" s="1" t="str">
@@ -659,7 +659,7 @@
       <c r="G6" s="1">
         <v>5</v>
       </c>
-      <c r="H6" s="16" t="s">
+      <c r="H6" s="10" t="s">
         <v>15</v>
       </c>
       <c r="I6" s="1" t="str">
@@ -672,7 +672,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="13" t="s">
         <v>0</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -686,154 +686,154 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="17">
+      <c r="C8" s="11">
         <v>1</v>
       </c>
-      <c r="D8" s="4" t="str">
+      <c r="D8" s="3" t="str">
         <f>D3&amp;"."&amp;D1&amp;"."&amp;D2</f>
         <v>192.168.19.14</v>
       </c>
-      <c r="E8" s="3" t="str">
+      <c r="E8" s="2" t="str">
         <f>D3&amp;"."&amp;D1&amp;"."&amp;0</f>
         <v>192.168.19.0</v>
       </c>
-      <c r="F8" s="13" t="str">
+      <c r="F8" s="15" t="str">
         <f>D3&amp;"."&amp;D1&amp;"."&amp;(D2+1)</f>
         <v>192.168.19.15</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="6" t="s">
+      <c r="A9" s="19"/>
+      <c r="B9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="18">
+      <c r="C9" s="12">
         <v>2</v>
       </c>
-      <c r="D9" s="7" t="str">
+      <c r="D9" s="5" t="str">
         <f>D3&amp;"."&amp;(D1+10)&amp;"."&amp;(D2)</f>
         <v>192.168.29.14</v>
       </c>
-      <c r="E9" s="6" t="str">
+      <c r="E9" s="4" t="str">
         <f>D3&amp;"."&amp;(D1+10)&amp;"."&amp;0</f>
         <v>192.168.29.0</v>
       </c>
-      <c r="F9" s="14"/>
+      <c r="F9" s="16"/>
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="9"/>
-      <c r="B10" s="10" t="s">
+      <c r="A10" s="20"/>
+      <c r="B10" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="20">
+      <c r="C10" s="14">
         <v>4</v>
       </c>
-      <c r="D10" s="7" t="str">
+      <c r="D10" s="5" t="str">
         <f>D3&amp;"."&amp;D1+29&amp;"."&amp;D2+3</f>
         <v>192.168.48.17</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="15"/>
+      <c r="F10" s="17"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="17">
+      <c r="C11" s="11">
         <v>2.2000000000000002</v>
       </c>
-      <c r="D11" s="17" t="str">
+      <c r="D11" s="11" t="str">
         <f>D3&amp;"."&amp;(D1+10)&amp;"."&amp;(D2+1)</f>
         <v>192.168.29.15</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="12"/>
+      <c r="F11" s="9"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="6" t="s">
+      <c r="A12" s="19"/>
+      <c r="B12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="19">
+      <c r="C12" s="13">
         <v>3</v>
       </c>
-      <c r="D12" s="7" t="str">
+      <c r="D12" s="5" t="str">
         <f>D3&amp;"."&amp;D1+15&amp;"."&amp;D2+1</f>
         <v>192.168.34.15</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F12" s="8" t="str">
+      <c r="F12" s="6" t="str">
         <f>D3&amp;"."&amp;D1+10&amp;"."&amp;D2+2</f>
         <v>192.168.29.16</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="9"/>
-      <c r="B13" s="10" t="s">
+      <c r="A13" s="20"/>
+      <c r="B13" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="18">
+      <c r="C13" s="12">
         <v>5</v>
       </c>
-      <c r="D13" s="6" t="str">
+      <c r="D13" s="4" t="str">
         <f>D3&amp;"."&amp;D1+11&amp;"."&amp;D2</f>
         <v>192.168.30.14</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F13" s="11"/>
+      <c r="F13" s="8"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="17">
+      <c r="C14" s="11">
         <v>4.2</v>
       </c>
-      <c r="D14" s="3" t="str">
+      <c r="D14" s="2" t="str">
         <f>D3&amp;"."&amp;D1+29&amp;"."&amp;D2+4</f>
         <v>192.168.48.18</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F14" s="12"/>
+      <c r="F14" s="9"/>
     </row>
     <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="9"/>
-      <c r="B15" s="10" t="s">
+      <c r="A15" s="20"/>
+      <c r="B15" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="20">
+      <c r="C15" s="14">
         <v>5.2</v>
       </c>
-      <c r="D15" s="10" t="str">
+      <c r="D15" s="7" t="str">
         <f>D3&amp;"."&amp;D1+11&amp;"."&amp;D2+1</f>
         <v>192.168.30.15</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E15" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F15" s="11"/>
+      <c r="F15" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>